<commit_message>
Started adding and testing unit spawns
</commit_message>
<xml_diff>
--- a/UnitDataSource.xlsx
+++ b/UnitDataSource.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13815" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UnitData" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="77">
   <si>
     <t>Name (string, required)</t>
   </si>
@@ -213,6 +213,45 @@
   </si>
   <si>
     <t>Fighter Group Size</t>
+  </si>
+  <si>
+    <t>Party Loss</t>
+  </si>
+  <si>
+    <t>Goblin Patrol</t>
+  </si>
+  <si>
+    <t>Snake Patrol</t>
+  </si>
+  <si>
+    <t>Slime Patrol</t>
+  </si>
+  <si>
+    <t>Skeleton Patrol</t>
+  </si>
+  <si>
+    <t>Goblin Army</t>
+  </si>
+  <si>
+    <t>Slime Army</t>
+  </si>
+  <si>
+    <t>Skeleton Army</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Unit Goal</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Bat Patrol</t>
+  </si>
+  <si>
+    <t>Serpent Army</t>
   </si>
 </sst>
 </file>
@@ -664,8 +703,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -708,57 +748,59 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1073,7 +1115,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,13 +1604,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B22"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1597,26 +1643,26 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1625,42 +1671,39 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4</v>
-      </c>
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1672,197 +1715,375 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>5</v>
-      </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>6</v>
-      </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>7</v>
-      </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>9</v>
-      </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
       <c r="B50" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>9</v>
+      </c>
+      <c r="B75" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1872,21 +2093,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1900,279 +2124,581 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <f>VLOOKUP(A2,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C2">
         <f>VLOOKUP(A2,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <f>CEILING(B2/UnitData!$E$3,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <f>VLOOKUP(A3,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(A3,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <f>CEILING(B3/UnitData!$E$3,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <f>VLOOKUP(A4,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C4">
         <f>VLOOKUP(A4,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <f>CEILING(B4/UnitData!$E$3,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <f>VLOOKUP(A5,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <f>VLOOKUP(A5,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <f>CEILING(B5/UnitData!$E$3,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <f>VLOOKUP(A6,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C6">
         <f>VLOOKUP(A6,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <f>CEILING(B6/UnitData!$E$3,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <f>VLOOKUP(A7,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C7">
         <f>VLOOKUP(A7,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <f>CEILING(B7/UnitData!$E$3,1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <f>VLOOKUP(A8,UnitData!$A$2:$E$12,4, FALSE)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C8">
         <f>VLOOKUP(A8,UnitData!$A$2:$E$12,5, FALSE)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <f>CEILING(B8/UnitData!$E$3,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <f>VLOOKUP(A9,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>120</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <f>CEILING(B9/UnitData!$E$3,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <f>VLOOKUP(A10,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>120</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <f>CEILING(B10/UnitData!$E$3,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <f>VLOOKUP(A11,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>120</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <f>CEILING(B11/UnitData!$E$3,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <f>VLOOKUP(A12,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>1200</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D12">
+        <f>CEILING(B12/UnitData!$E$3,1)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <f>VLOOKUP(A13,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>1200</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D13">
+        <f>CEILING(B13/UnitData!$E$3,1)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <f>VLOOKUP(A14,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>1200</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D14">
+        <f>CEILING(B14/UnitData!$E$3,1)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <f>VLOOKUP(A15,UnitData!$A$2:$E$12,4, FALSE)</f>
+        <v>1200</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15,UnitData!$A$2:$E$12,5, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D15">
+        <f>CEILING(B15/UnitData!$E$3,1)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1">
+        <f>SUM(B2:B19)</f>
+        <v>6000</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(C2:C19)</f>
+        <v>450</v>
+      </c>
+      <c r="D20" s="1">
+        <f>SUM(D2:D19)</f>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4">
+        <f>UnitData!$D$3 / SUM(C2:C19)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="5">
+        <f>C20/UnitData!D2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <f>A25*UnitData!$D$3</f>
+        <v>150</v>
+      </c>
+      <c r="C25">
+        <f>A25 * UnitData!$E$3</f>
+        <v>18</v>
+      </c>
+      <c r="D25" s="3">
+        <f>$D$20/A25</f>
+        <v>338</v>
+      </c>
+      <c r="E25" s="3">
+        <f>D25/$C$21</f>
+        <v>1014</v>
+      </c>
+      <c r="F25" s="6">
+        <f>E25/A25</f>
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <f>A26*UnitData!$D$3</f>
+        <v>750</v>
+      </c>
+      <c r="C26">
+        <f>A26 * UnitData!$E$3</f>
+        <v>90</v>
+      </c>
+      <c r="D26" s="3">
+        <f>$D$20/A26</f>
+        <v>67.599999999999994</v>
+      </c>
+      <c r="E26" s="3">
+        <f>D26/$C$21</f>
+        <v>202.79999999999998</v>
+      </c>
+      <c r="F26" s="6">
+        <f>E26/A26</f>
+        <v>40.559999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <f>A27*UnitData!$D$3</f>
+        <v>1500</v>
+      </c>
+      <c r="C27">
+        <f>A27 * UnitData!$E$3</f>
+        <v>180</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" ref="D27:D31" si="0">$D$20/A27</f>
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" ref="E27:E31" si="1">D27/$C$21</f>
+        <v>101.39999999999999</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" ref="F27:F31" si="2">E27/A27</f>
+        <v>10.139999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <f>A28*UnitData!$D$3</f>
+        <v>2250</v>
+      </c>
+      <c r="C28">
+        <f>A28 * UnitData!$E$3</f>
+        <v>270</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" ref="D28" si="3">$D$20/A28</f>
+        <v>22.533333333333335</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>67.600000000000009</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" ref="F28" si="4">E28/A28</f>
+        <v>4.5066666666666668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <f>A29*UnitData!$D$3</f>
+        <v>3750</v>
+      </c>
+      <c r="C29">
+        <f>A29 * UnitData!$E$3</f>
+        <v>450</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>13.52</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>40.56</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6224000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <f>A30*UnitData!$D$3</f>
+        <v>7500</v>
+      </c>
+      <c r="C30">
+        <f>A30 * UnitData!$E$3</f>
+        <v>900</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>6.76</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>20.28</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="2"/>
+        <v>0.40560000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>100</v>
+      </c>
+      <c r="B31">
+        <f>A31*UnitData!$D$3</f>
+        <v>15000</v>
+      </c>
+      <c r="C31">
+        <f>A31 * UnitData!$E$3</f>
+        <v>1800</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>3.38</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>10.14</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="2"/>
+        <v>0.1014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="1">
-        <f>SUM(B2:B10)</f>
-        <v>420</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" ref="C11:D11" si="0">SUM(C2:C10)</f>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="4">
-        <f>UnitData!$D$3 / SUM(C2:C10)</f>
-        <v>2.1428571428571428</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="5">
-        <f>C11/UnitData!D2</f>
-        <v>0.93333333333333335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <f>A16*UnitData!$D$3</f>
-        <v>750</v>
-      </c>
-      <c r="C16">
-        <f>A16 * UnitData!$E$3</f>
-        <v>90</v>
-      </c>
-      <c r="D16">
-        <f>$D$11/A16</f>
-        <v>5.6</v>
-      </c>
-      <c r="E16" s="3">
-        <f>D16/$C$12</f>
-        <v>2.6133333333333333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <f>A17*UnitData!$D$3</f>
-        <v>1500</v>
-      </c>
-      <c r="C17">
-        <f>A17 * UnitData!$E$3</f>
-        <v>180</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ref="D17:D20" si="1">$D$11/A17</f>
-        <v>2.8</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" ref="E17:E20" si="2">D17/$C$12</f>
-        <v>1.3066666666666666</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="C45">
         <v>25</v>
       </c>
-      <c r="B18">
-        <f>A18*UnitData!$D$3</f>
-        <v>3750</v>
-      </c>
-      <c r="C18">
-        <f>A18 * UnitData!$E$3</f>
-        <v>450</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="2"/>
-        <v>0.52266666666666672</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47">
         <v>50</v>
-      </c>
-      <c r="B19">
-        <f>A19*UnitData!$D$3</f>
-        <v>7500</v>
-      </c>
-      <c r="C19">
-        <f>A19 * UnitData!$E$3</f>
-        <v>900</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="2"/>
-        <v>0.26133333333333336</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>100</v>
-      </c>
-      <c r="B20">
-        <f>A20*UnitData!$D$3</f>
-        <v>15000</v>
-      </c>
-      <c r="C20">
-        <f>A20 * UnitData!$E$3</f>
-        <v>1800</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="2"/>
-        <v>0.13066666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More spawner changes and testing
</commit_message>
<xml_diff>
--- a/UnitDataSource.xlsx
+++ b/UnitDataSource.xlsx
@@ -1606,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,17 +1652,17 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>